<commit_message>
title und struktur angepasst
</commit_message>
<xml_diff>
--- a/considerations to http locations.xlsx
+++ b/considerations to http locations.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Requirements" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Location</t>
   </si>
@@ -88,6 +88,30 @@
   </si>
   <si>
     <t>www.sitex.com/n/1201</t>
+  </si>
+  <si>
+    <t>http://www.google.de/int/a/b</t>
+  </si>
+  <si>
+    <t>int/a/b</t>
+  </si>
+  <si>
+    <t>http://www.google.de/int/a/b/</t>
+  </si>
+  <si>
+    <t>int/a/b/</t>
+  </si>
+  <si>
+    <t>www.google.de/int/a/b</t>
+  </si>
+  <si>
+    <t>www.google.de/int/a/b/</t>
+  </si>
+  <si>
+    <t>einheitliche Überschriften</t>
+  </si>
+  <si>
+    <t>Edit / show einheitlich</t>
   </si>
 </sst>
 </file>
@@ -439,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,24 +633,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>